<commit_message>
1. part ID cannot contain "_" 2. Export excel for close repair ticket
</commit_message>
<xml_diff>
--- a/report_template/closedRepairTicket.xlsx
+++ b/report_template/closedRepairTicket.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>案件編號</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -64,6 +64,16 @@
   <si>
     <t>完成日期</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>故障說明</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>維修經過</t>
+  </si>
+  <si>
+    <t>結果</t>
   </si>
 </sst>
 </file>
@@ -483,7 +493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
@@ -492,10 +502,11 @@
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="10.125" customWidth="1"/>
-    <col min="10" max="10" width="14.375" customWidth="1"/>
+    <col min="10" max="12" width="11.375" customWidth="1"/>
+    <col min="13" max="13" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -506,8 +517,11 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,12 +550,21 @@
         <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>